<commit_message>
Updating for live website
</commit_message>
<xml_diff>
--- a/Database Construction scripts/Restructured ESEP Database - Neel preliminary data.xlsx
+++ b/Database Construction scripts/Restructured ESEP Database - Neel preliminary data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabi &amp; Teaching Resources" sheetId="1" state="visible" r:id="rId2"/>
@@ -400,7 +400,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Name </t>
+    <t xml:space="preserve">Name </t>
   </si>
   <si>
     <t xml:space="preserve">Organization Type</t>
@@ -1373,19 +1373,19 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2558139534884"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.78604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.7209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="92.7906976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.90697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.3953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.7023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="95.4976744186046"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,12 +1573,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="42.0883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="110.386046511628"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="43.3162790697674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="113.711627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" s="48" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,15 +1704,15 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="112.111627906977"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="115.553488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,10 +1824,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.7441860465116"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="35.6883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.5906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="36.7953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,15 +1995,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="63.3767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="12.8"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="14.7674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="9.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="15.1348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2209,24 +2209,24 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="63.3767441860465"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="12.8"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="14" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="51.1953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="14" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="52.7953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.1813953488372"/>
   </cols>
   <sheetData>
-    <row r="1" s="17" customFormat="true" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="17" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>102</v>
       </c>
@@ -2397,15 +2397,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="63.3767441860465"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="14" width="12.8"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="51.1953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="14" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="10" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="14" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="52.7953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="14" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="10" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="53" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6652,12 +6652,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="59.5627906976744"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="67.5627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="56.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="22.3953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="69.6511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" s="26" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6806,11 +6806,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="24" width="60.5488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="101.525581395349"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="24" width="62.2697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="104.604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" s="30" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6956,13 +6956,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="71.9906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="85.4046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="32" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="74.2046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="87.9906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="32" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" s="38" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7129,10 +7129,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="32" width="63.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="32" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="32" width="65.0976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="32" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adding support for new data structure, profiles
</commit_message>
<xml_diff>
--- a/Database Construction scripts/Restructured ESEP Database - Neel preliminary data.xlsx
+++ b/Database Construction scripts/Restructured ESEP Database - Neel preliminary data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabi &amp; Teaching Resources" sheetId="1" state="visible" r:id="rId2"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="271">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -397,475 +397,475 @@
     <t xml:space="preserve">www.europarl.europa.eu/stoa/cms/home/activities/mepscientist</t>
   </si>
   <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Science &amp; Technology Policy Fellowships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Science &amp; Technology Policy Fellowships (STPF) provide opportunities to outstanding scientists and engineers to learn first-hand about policymaking and contribute their knowledge and analytical skills in the policy realm. Fellows serve yearlong assignments in the federal government and represent a broad range of backgrounds, disciplines, and career stages. Each year, STPF adds to a growing corps over 3,000 strong of policy-savvy leaders working across academia, government, nonprofits, and industry to serve the nation and citizens around the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Association for the Advancement of Science (AAAS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Governmental Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Graduate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/stpf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAS John Bahcall Public Policy Fellowship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The John N. Bahcall Public Policy Fellowship was created in 2006, in collaboration with Neta Bahcall, to provide an opportunity for early-career astronomers to gain experience in the world of science policy and to augment the advocacy programs of the society. The Bahcall Fellowship is currently a one-year postdoctoral level appointment, renewable for a second year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Astronomical Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aas.org/programs/john-bahcall-public-policy-fellowship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACS Public Policy Fellowships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ACS Congressional and Science Policy Fellowship Programs are designed to address both these concerns. The programs provide a unique opportunity for ACS members to gain practical experience and insights into public policy by working on Capitol Hill or at ACS in Washington, DC. Fellows may be entry-level PhDs or experienced professionals from academia, industry, or non-profits. Former fellows have covered issues as diverse as federal funding for scientific research, science education, and health policy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Chemical Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.acs.org/content/acs/en/policy/policyfellowships.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AERA Congressional Fellowship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goals of the fellowship are: (1) to contribute to the effective use of scientiﬁc knowledge about education in the formation of public policy; (2) to educate the scientiﬁc community about the development of public policy; and (3) to establish a more effective liaison between education researchers and federal policymakers. Following a two-week science policy orientation program, the AERA fellow will begin work as a resident scholar within a congressional office. AERA Congressional Fellows will benefit from on-going professional development and networking opportunities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Educational Research Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aera.net/Research-Policy-Advocacy/AERA-Congressional-Fellowship </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizenship Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Science Policy Internships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Science Policy Internships are offered in Government Relations, Science &amp; Diplomacy, Scientific Responsibility, Human Rights and Law, and in Science, Ethics an Religion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/page/internship-opportunities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Association for the Advancement of Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-governmental Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGI Geoscience Policy Internship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Geoscience Policy program represents the shared interests of the geoscience community in Washington, D.C., and actively works with Congress and federal agencies to foster better communication and public policy for the geosciences in areas including water, energy and mineral resources, natural hazards, environmental protection, and federal funding for geoscience research and education. AGI seeks outstanding geoscience or engineering students or recent graduates (Bachelor's or Master's level) with a strong interest in federal science policy. Interns will hone their writing and web publishing skills, while gaining first-hand policy experience and improving their understanding of the legislative process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.americangeosciences.org/policy/internships-and-fellowships#PolicyInternship </t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Geosciences Institute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachlor's or Master's student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APLU Governmental Affairs Internship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Congressional and Governmental Affairs (CGA) office of APLU is focused on representing university interests before Congress and the Executive Branch on many of today’s cutting edge issues. Topics range from student financial aid and scientific research, to tax policy and appropriations, to energy policy and international development. Interns will work with the Congressional and Governmental Affairs staff to promote the association’s agenda before the federal government.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aplu.org/members/jobs-at-aplu-and-member-institutions/employment-opportunities/governmental-affairs-internship </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association of Public and Land-grant Universities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current student or recent graduate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASME Washington Internships for Students of Engineering (WISE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each year, the WISE sponsoring societies select outstanding engineering students from among their memberships to participate in the nine-week WISE program in Washington. Students discover how government officials make decisions on complex technological issues, while at the same time, learning how engineers and scientists can contribute to the legislative process and regulatory decision-making.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.wise-intern.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Society of Mechanical Engineers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineering, U.S. Citizenship, Permanent Residency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORGANIZER(S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Annual Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AAAS Annual Meeting is one of the most widely recognized and reported interdisciplinary scientific events, encompassing the breadth of the sciences as well as education, engineering, and technology. It is a major attraction for the scientific, business, NGO, media, and policy-maker communities concerned about the interaction of science and technology with society.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/annual-meeting/archives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Forum on Science and Technology Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The annual AAAS Forum on Science and Technology Policy is an excellent conference for people interested in public policy issues facing the science, engineering, and higher education communities. Since 1976, it has provided a mechanism by which individuals interested in science policy could go to learn what is happening and what is likely to happen in the coming year on the federal budget and the growing number of policy issues that affect researchers and their institutions. The forum is held in the spring, usually in late April or early May.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/page/forum-science-technology-policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian Science Policy Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian Science Policy Centre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Canadian Science Policy Conference is an ideal event for researchers across all sectors, industrial R&amp;D managers and senior management from the private sector, government policy-makers (federal, territorial, provincial, and local), research granting agencies and funding bodies, non-governmental organizations, writers and journalists, communications and government relations professionals, scientific associations, students and trainees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sciencepolicy.ca/conferences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CILAC: Open Science Forum for Latin America and Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNESCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Open Science Forum for Latin America and the Caribbean has construed itself as a key regional space for debates and exchanges and is organized every two years, alternating in distinct cities throughout the region. It seeks to establish itself as a platform for the outlining of common positions and aspirations for a scientific, technological, and innovation agenda supporting sustainable development whilst simultaneously giving the region a strong voice in the global scope of the World Science Forum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://forocilac.org/en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EuroScience Open Forum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euroscience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESOF (EuroScience Open Forum) is the largest interdisciplinary science meeting in Europe. It is dedicated to scientific research and innovation and offers a unique framework for interaction and debate for scientists, innovators, policy makers, business people and the general public. Created in 2004 by EuroScience, this biennial European forum brings together over 4 000 researchers, educators, business actors, policy makers and journalists from all over the world to discuss breakthroughs in science. More than 40% of the participants are students and young researchers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euorpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.esof.eu/en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INGSA Conferences and Meetings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Network for Government Science Advice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INGSA convenes an international conference every two years on the issues of science advice to governments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ingsa.org/events/ingsa-conferences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan Alda-Kavli Science Communication Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alan Alda Center for Communicating Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Alan Alda Center for Communicating Science serves scientists, medical professionals, students, and the public with opportunities to explore, learn, and practice communicating effectively about science and medicine. We are an online resource for information and training in science communication, uniting research and methodology from institutions and individuals throughout the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aldakavlilearningcenter.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalyzing Advocacy in Science and Engineering (CASE) Workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper-class undergraduate &amp; graduate students: Join us for a three-and-a-half-day program in DC to learn about Congress, the federal budget process, and effective science communication. Students will have an opportunity to meet with their Members of Congress or congressional staff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aaas.org/page/about-case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leadership Seminar in Science &amp; Technology Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AAAS Leadership Seminar in Science and Technology Policy is a "crash course" in science and technology (S&amp;T) policy, designed for those who need to know how S&amp;T policy works. It is modeled after the highly acclaimed orientation program that AAAS provides for its new S&amp;T Policy Fellows each fall, but distills the key material into 4 1/2 days instead of two weeks. Space is limited to only 30 to 35 participants ‐ the small group setting provides an ideal opportunity to learn about the challenges and solutions of S&amp;T policy from the experts. Join AAAS to learn firsthand from key people in S&amp;T policy, in settings ranging from Capitol Hill to White House staff offices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aaas.org/page/science-technology-policy-leadership-seminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Communicating Science Workshops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAAS Communicating Science workshops, developed by the Center for Public Engagement with Science and Technology, are specifically designed to address the needs of scientists and engineers to communicate scientific or technical information in a variety of public and professional interactions, such as media interviews, writing grant proposals, discussing ideas with students, testifying before Congress, or participating in public forums.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/pes/communicating-science-workshops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Diplomacy: An Online Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This one-hour course, hosted by Dr. Marga Gual Soler and Dr. Tom Wang of the AAAS Center for Science Diplomacy, is the first ever online course fully dedicated to science diplomacy. It includes the basic definitions and frameworks of science diplomacy, its evolution in history, and several case studies with interviews with top practitioners in the field. Join us and learn all about the connections between science and diplomacy throughout the ages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.aaas.org/scidip-online-course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer Policy Colloquium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Meteorological Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each year, the AMS Summer Policy Colloquium brings a select group to Washington, D.C. for an intense, ten-day immersion in science policy. Graduate students, faculty and professionals in the field of earth and atmospheric sciences and their applications form a cohort that tackles hands-on exercises, hears from dozens of prominent experts and forges strong professional networking connections. The Summer Policy Colloquium is a career-shaping experience. By arming tomorrow's leaders with expertise in the policy process, the science community will be more engaged with decision makers, helping ensure that society's policy choices take full advantage of available scientific knowledge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.ametsoc.org/ams/index.cfm/policy/summer-policy-colloquium/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membership Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEOGRAPHIC SCOPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 Women Scientists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 Women Scientists is a grassroots organization started by four women who met in graduate school at CU Boulder and who maintained friendships and collaborations after jobs and life took them away from Boulder. Immediately following the November 2016 election, we published an open letter re-affirming our commitment to speak up for science and for women, minorities, immigrants, people with disabilities, and LGBTQIA. 500 Women Scientists works to build communities and foster real change that comes from small groups, not large crowds. Our Local Pods help create those deep roots through strong, personal relationships. Local Pods are where members meet regularly, develop a support network, make strategic plans, and take action. Pods focus on issues that resonate in their communities, rooted in our mission and values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://500womenscientists.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa Evidence Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Africa Evidence Network (AEN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Africa Evidence Network (AEN) is a community of people who work in Africa and have an interest in evidence, its production and use in decision-making. The Network is supported by the Africa Centre for Evidence within the University of Johannesburg and includes researchers, practitioners and policy-makers from universities, civil society and government.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.africaevidencenetwork.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">African Technology Policy Studies Network (ATPS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ATPS is a trans-disciplinary network of researchers, policymakers, private sector actors and the civil society that promote the generation, dissemination, use and mastery of science, technology and innovation for African development, environmental sustainability and global inclusion. Today, the ATPS has over 1,500 members and 3000 stakeholders in over 51 countries in 5 continents with institutional partnerships worldwide. We implement our programs through members in national chapters established in 30 countries (27 in Africa and 3 Diaspora chapters in the Australia, United States of America, and United Kingdom) with its secretariat in Nairobi Kenya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.atpsnet.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engaging Scientists and Engineers in Policy (ESEP) Coalition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Engaging Scientists &amp; Engineers in Policy (ESEP) Coalition is an ad hoc alliance of organizations that have joined together to empower scientists and engineers to effectively engage in the policy making process at all levels of government (federal, state and local). ​ESEP serves as a resource one-stop-shop, a communication forum, networking opportunity and as an engagement vehicle for science &amp; technology policy stakeholders. Interested or already involved with S&amp;T policy? Join us!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.science-engage.org/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU Agencies Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Union Agencies Network (EUAN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUAN is comprised of 45 Agencies and Joint Undertakings. The Agencies which are spread across Europe work in a wide range of policy areas, from health and environment, to migration and security, to business and innovation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://euagencies.eu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friends of Joe's Big Idea </t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Public Radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe's Big Idea (JBI) was started by NPR Science Correspondent Joe Palca in 2012, in an effort to tell stories about the processes of science and invention. During his travels, Joe interacted with many young scientists who wanted to become better communicators. So, Joe started the group - Friends Of Joe's Big Idea (FOJBIs).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.npr.org/2017/08/24/537735624/friends-of-joes-big-idea-fojbis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating Science: Tools for Scientists and Engineers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From the AAAS Center for Public Engagement with Science &amp; Technology, this tool-kit provides scientists and scientific institutions of all academic disciplines with the resources they need to have meaningful conversations with the public.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aaas.org/comm-toolkit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Advocacy Tool-Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Psychological Association </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On these pages, find simple, effective tools that explain the hot issues. The how-to’s of talking to your representatives, visiting them in your district and, if necessary, on Capitol Hill. What’s been done before. What you can do as soon as today. And how we will help, every step.​</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://advocacy.apascience.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Practices for Messaging Before, During, and After the March for Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have received several questions from ESEP members regarding best practices for messaging before, during, and after the March for Science. This guide addresses some of the questions we have received along with some thoughts and advice in response to them. We hope ESEP members and those that would like to engage in science policy who might have been inspired by the March for Science find this information useful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://science-engage.org/uploads/3/4/9/0/34906793/esep_-_messaging_for_the_march_for_science.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy and Advocacy Tool-Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federation of American Societies for Experimental Biology (FASEB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASEB represents more than 125,000 scientists and engineers through collaborative advocacy with constituent societies. FASEB's top priority is urging Congress to provide sustainable and predictable federal funding for scientific research.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://faseb.org/Science-Policy-and-Advocacy/Become-an-Advocate/Advocacy-Tool-Kit.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Coalition Tool-Kit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Science Coalition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Established in 1994, the Science Coalition is a nonprofit, nonpartisan organization of more than 50 of the nation’s leading public and private research universities. It is dedicated to sustaining the federal government’s investment in basic scientific research as a means to stimulate the economy, spur innovation and drive America’s global competitiveness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.sciencecoalition.org/mission-and-members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvard GSAS Science Policy Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvard University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Harvard GSAS Science Policy Group is composed of graduate students interested in the intersection between science and policy. We work to engage Harvard science students by hosting networking events, chats with science policy experts, courses, career panels, local trips to government agencies, writing and research opportunities, and an annual visit to Washington, D.C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://projects.iq.harvard.edu/sciencepolicy/home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT Science Policy Initiative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MIT Science Policy Initiative, founded in 2007, is a group of graduate (and some undergraduate) students who work closely with MIT Faculty, the MIT Washington DC Office, and other science policy advocates to better understand how scientists can play a central role in the framing of science and technology policy legislation and public discourse. We strive to create better scientists and engineers as well as a better society through rigorous research and authentic engagement with public policy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mitspi.squarespace.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science and Education Policy Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weill Cornell Medicine, The Rockefeller University, and Memorial Sloan Kettering Cancer Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Science &amp; Education Policy Association (SEPA) is a student-run organization founded at the Tri-Institute – Weill Cornell Medicine, The Rockefeller University, and Memorial Sloan Kettering Cancer Center – aiming to facilitate the interaction between scientists and the world of science policy. Launched in 2016 by Sarah Qamar and Dane Samilo, SEPA is continuing its work to advocate and raise awareness for the need for policy engagement within the scientific community.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sepanyc.org/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fletcher Science Diplomacy Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tufts University, Fletcher School </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Fletcher Science Diplomacy club was founded in September 2016. It maintains close ties to the Science Diplomacy Center (Tufts University) and the Science Diplomacy Education Network (AAAS Center for Science Diplomacy). The club aims to raise awareness of the growing field of science diplomacy, highlighting the role of science in informing sound policy-making, solving global challenges and improving international relations. The club provides a forum for students, at the Fletcher School and beyond, to explore and understand issues at the intersection of science and international relations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sites.tufts.edu/scidipclub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Policy Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of California, San Francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are a registered campus organization (RCO) dedicated to educating our students and postdocs about science policy issues as well as taking action to support science advocacy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.facebook.com/UcsfSciencePolicyGroup</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citizen Requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Degree Requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Science &amp; Technology Policy Fellowships</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Science &amp; Technology Policy Fellowships (STPF) provide opportunities to outstanding scientists and engineers to learn first-hand about policymaking and contribute their knowledge and analytical skills in the policy realm. Fellows serve yearlong assignments in the federal government and represent a broad range of backgrounds, disciplines, and career stages. Each year, STPF adds to a growing corps over 3,000 strong of policy-savvy leaders working across academia, government, nonprofits, and industry to serve the nation and citizens around the world.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Association for the Advancement of Science (AAAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Governmental Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Post Graduate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/stpf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAS John Bahcall Public Policy Fellowship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The John N. Bahcall Public Policy Fellowship was created in 2006, in collaboration with Neta Bahcall, to provide an opportunity for early-career astronomers to gain experience in the world of science policy and to augment the advocacy programs of the society. The Bahcall Fellowship is currently a one-year postdoctoral level appointment, renewable for a second year.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Astronomical Society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aas.org/programs/john-bahcall-public-policy-fellowship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACS Public Policy Fellowships</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ACS Congressional and Science Policy Fellowship Programs are designed to address both these concerns. The programs provide a unique opportunity for ACS members to gain practical experience and insights into public policy by working on Capitol Hill or at ACS in Washington, DC. Fellows may be entry-level PhDs or experienced professionals from academia, industry, or non-profits. Former fellows have covered issues as diverse as federal funding for scientific research, science education, and health policy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Chemical Society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.acs.org/content/acs/en/policy/policyfellowships.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AERA Congressional Fellowship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The goals of the fellowship are: (1) to contribute to the effective use of scientiﬁc knowledge about education in the formation of public policy; (2) to educate the scientiﬁc community about the development of public policy; and (3) to establish a more effective liaison between education researchers and federal policymakers. Following a two-week science policy orientation program, the AERA fellow will begin work as a resident scholar within a congressional office. AERA Congressional Fellows will benefit from on-going professional development and networking opportunities.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Educational Research Association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aera.net/Research-Policy-Advocacy/AERA-Congressional-Fellowship </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citizenship Requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Science Policy Internships</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Science Policy Internships are offered in Government Relations, Science &amp; Diplomacy, Scientific Responsibility, Human Rights and Law, and in Science, Ethics an Religion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/page/internship-opportunities </t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Association for the Advancement of Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-governmental Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGI Geoscience Policy Internship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Geoscience Policy program represents the shared interests of the geoscience community in Washington, D.C., and actively works with Congress and federal agencies to foster better communication and public policy for the geosciences in areas including water, energy and mineral resources, natural hazards, environmental protection, and federal funding for geoscience research and education. AGI seeks outstanding geoscience or engineering students or recent graduates (Bachelor's or Master's level) with a strong interest in federal science policy. Interns will hone their writing and web publishing skills, while gaining first-hand policy experience and improving their understanding of the legislative process.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.americangeosciences.org/policy/internships-and-fellowships#PolicyInternship </t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Geosciences Institute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bachlor's or Master's student</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APLU Governmental Affairs Internship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Congressional and Governmental Affairs (CGA) office of APLU is focused on representing university interests before Congress and the Executive Branch on many of today’s cutting edge issues. Topics range from student financial aid and scientific research, to tax policy and appropriations, to energy policy and international development. Interns will work with the Congressional and Governmental Affairs staff to promote the association’s agenda before the federal government.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aplu.org/members/jobs-at-aplu-and-member-institutions/employment-opportunities/governmental-affairs-internship </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association of Public and Land-grant Universities </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current student or recent graduate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASME Washington Internships for Students of Engineering (WISE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each year, the WISE sponsoring societies select outstanding engineering students from among their memberships to participate in the nine-week WISE program in Washington. Students discover how government officials make decisions on complex technological issues, while at the same time, learning how engineers and scientists can contribute to the legislative process and regulatory decision-making.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.wise-intern.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Society of Mechanical Engineers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineering, U.S. Citizenship, Permanent Residency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORGANIZER(S)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Annual Meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The AAAS Annual Meeting is one of the most widely recognized and reported interdisciplinary scientific events, encompassing the breadth of the sciences as well as education, engineering, and technology. It is a major attraction for the scientific, business, NGO, media, and policy-maker communities concerned about the interaction of science and technology with society.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/annual-meeting/archives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Forum on Science and Technology Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The annual AAAS Forum on Science and Technology Policy is an excellent conference for people interested in public policy issues facing the science, engineering, and higher education communities. Since 1976, it has provided a mechanism by which individuals interested in science policy could go to learn what is happening and what is likely to happen in the coming year on the federal budget and the growing number of policy issues that affect researchers and their institutions. The forum is held in the spring, usually in late April or early May.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/page/forum-science-technology-policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canadian Science Policy Conference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canadian Science Policy Centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Canadian Science Policy Conference is an ideal event for researchers across all sectors, industrial R&amp;D managers and senior management from the private sector, government policy-makers (federal, territorial, provincial, and local), research granting agencies and funding bodies, non-governmental organizations, writers and journalists, communications and government relations professionals, scientific associations, students and trainees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://sciencepolicy.ca/conferences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CILAC: Open Science Forum for Latin America and Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNESCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Open Science Forum for Latin America and the Caribbean has construed itself as a key regional space for debates and exchanges and is organized every two years, alternating in distinct cities throughout the region. It seeks to establish itself as a platform for the outlining of common positions and aspirations for a scientific, technological, and innovation agenda supporting sustainable development whilst simultaneously giving the region a strong voice in the global scope of the World Science Forum.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://forocilac.org/en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EuroScience Open Forum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euroscience</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESOF (EuroScience Open Forum) is the largest interdisciplinary science meeting in Europe. It is dedicated to scientific research and innovation and offers a unique framework for interaction and debate for scientists, innovators, policy makers, business people and the general public. Created in 2004 by EuroScience, this biennial European forum brings together over 4 000 researchers, educators, business actors, policy makers and journalists from all over the world to discuss breakthroughs in science. More than 40% of the participants are students and young researchers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Euorpe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.esof.eu/en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INGSA Conferences and Meetings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Network for Government Science Advice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INGSA convenes an international conference every two years on the issues of science advice to governments.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ingsa.org/events/ingsa-conferences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Alda-Kavli Science Communication Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alan Alda Center for Communicating Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Alan Alda Center for Communicating Science serves scientists, medical professionals, students, and the public with opportunities to explore, learn, and practice communicating effectively about science and medicine. We are an online resource for information and training in science communication, uniting research and methodology from institutions and individuals throughout the world.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aldakavlilearningcenter.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalyzing Advocacy in Science and Engineering (CASE) Workshop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper-class undergraduate &amp; graduate students: Join us for a three-and-a-half-day program in DC to learn about Congress, the federal budget process, and effective science communication. Students will have an opportunity to meet with their Members of Congress or congressional staff.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.aaas.org/page/about-case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leadership Seminar in Science &amp; Technology Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The AAAS Leadership Seminar in Science and Technology Policy is a "crash course" in science and technology (S&amp;T) policy, designed for those who need to know how S&amp;T policy works. It is modeled after the highly acclaimed orientation program that AAAS provides for its new S&amp;T Policy Fellows each fall, but distills the key material into 4 1/2 days instead of two weeks. Space is limited to only 30 to 35 participants ‐ the small group setting provides an ideal opportunity to learn about the challenges and solutions of S&amp;T policy from the experts. Join AAAS to learn firsthand from key people in S&amp;T policy, in settings ranging from Capitol Hill to White House staff offices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.aaas.org/page/science-technology-policy-leadership-seminar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Communicating Science Workshops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAAS Communicating Science workshops, developed by the Center for Public Engagement with Science and Technology, are specifically designed to address the needs of scientists and engineers to communicate scientific or technical information in a variety of public and professional interactions, such as media interviews, writing grant proposals, discussing ideas with students, testifying before Congress, or participating in public forums.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/pes/communicating-science-workshops</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science Diplomacy: An Online Course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This one-hour course, hosted by Dr. Marga Gual Soler and Dr. Tom Wang of the AAAS Center for Science Diplomacy, is the first ever online course fully dedicated to science diplomacy. It includes the basic definitions and frameworks of science diplomacy, its evolution in history, and several case studies with interviews with top practitioners in the field. Join us and learn all about the connections between science and diplomacy throughout the ages.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.aaas.org/scidip-online-course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summer Policy Colloquium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Meteorological Society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each year, the AMS Summer Policy Colloquium brings a select group to Washington, D.C. for an intense, ten-day immersion in science policy. Graduate students, faculty and professionals in the field of earth and atmospheric sciences and their applications form a cohort that tackles hands-on exercises, hears from dozens of prominent experts and forges strong professional networking connections. The Summer Policy Colloquium is a career-shaping experience. By arming tomorrow's leaders with expertise in the policy process, the science community will be more engaged with decision makers, helping ensure that society's policy choices take full advantage of available scientific knowledge.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.ametsoc.org/ams/index.cfm/policy/summer-policy-colloquium/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Membership Fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEOGRAPHIC SCOPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500 Women Scientists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500 Women Scientists is a grassroots organization started by four women who met in graduate school at CU Boulder and who maintained friendships and collaborations after jobs and life took them away from Boulder. Immediately following the November 2016 election, we published an open letter re-affirming our commitment to speak up for science and for women, minorities, immigrants, people with disabilities, and LGBTQIA. 500 Women Scientists works to build communities and foster real change that comes from small groups, not large crowds. Our Local Pods help create those deep roots through strong, personal relationships. Local Pods are where members meet regularly, develop a support network, make strategic plans, and take action. Pods focus on issues that resonate in their communities, rooted in our mission and values.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://500womenscientists.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Africa Evidence Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Africa Evidence Network (AEN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Africa Evidence Network (AEN) is a community of people who work in Africa and have an interest in evidence, its production and use in decision-making. The Network is supported by the Africa Centre for Evidence within the University of Johannesburg and includes researchers, practitioners and policy-makers from universities, civil society and government.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.africaevidencenetwork.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">African Technology Policy Studies Network (ATPS) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ATPS is a trans-disciplinary network of researchers, policymakers, private sector actors and the civil society that promote the generation, dissemination, use and mastery of science, technology and innovation for African development, environmental sustainability and global inclusion. Today, the ATPS has over 1,500 members and 3000 stakeholders in over 51 countries in 5 continents with institutional partnerships worldwide. We implement our programs through members in national chapters established in 30 countries (27 in Africa and 3 Diaspora chapters in the Australia, United States of America, and United Kingdom) with its secretariat in Nairobi Kenya.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.atpsnet.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engaging Scientists and Engineers in Policy (ESEP) Coalition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Engaging Scientists &amp; Engineers in Policy (ESEP) Coalition is an ad hoc alliance of organizations that have joined together to empower scientists and engineers to effectively engage in the policy making process at all levels of government (federal, state and local). ​ESEP serves as a resource one-stop-shop, a communication forum, networking opportunity and as an engagement vehicle for science &amp; technology policy stakeholders. Interested or already involved with S&amp;T policy? Join us!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.science-engage.org/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU Agencies Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Union Agencies Network (EUAN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUAN is comprised of 45 Agencies and Joint Undertakings. The Agencies which are spread across Europe work in a wide range of policy areas, from health and environment, to migration and security, to business and innovation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://euagencies.eu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friends of Joe's Big Idea </t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Public Radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joe's Big Idea (JBI) was started by NPR Science Correspondent Joe Palca in 2012, in an effort to tell stories about the processes of science and invention. During his travels, Joe interacted with many young scientists who wanted to become better communicators. So, Joe started the group - Friends Of Joe's Big Idea (FOJBIs).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.npr.org/2017/08/24/537735624/friends-of-joes-big-idea-fojbis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communicating Science: Tools for Scientists and Engineers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From the AAAS Center for Public Engagement with Science &amp; Technology, this tool-kit provides scientists and scientific institutions of all academic disciplines with the resources they need to have meaningful conversations with the public.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.aaas.org/comm-toolkit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science Advocacy Tool-Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American Psychological Association </t>
-  </si>
-  <si>
-    <t xml:space="preserve">On these pages, find simple, effective tools that explain the hot issues. The how-to’s of talking to your representatives, visiting them in your district and, if necessary, on Capitol Hill. What’s been done before. What you can do as soon as today. And how we will help, every step.​</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://advocacy.apascience.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Practices for Messaging Before, During, and After the March for Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We have received several questions from ESEP members regarding best practices for messaging before, during, and after the March for Science. This guide addresses some of the questions we have received along with some thoughts and advice in response to them. We hope ESEP members and those that would like to engage in science policy who might have been inspired by the March for Science find this information useful.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://science-engage.org/uploads/3/4/9/0/34906793/esep_-_messaging_for_the_march_for_science.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy and Advocacy Tool-Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Federation of American Societies for Experimental Biology (FASEB) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FASEB represents more than 125,000 scientists and engineers through collaborative advocacy with constituent societies. FASEB's top priority is urging Congress to provide sustainable and predictable federal funding for scientific research.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://faseb.org/Science-Policy-and-Advocacy/Become-an-Advocate/Advocacy-Tool-Kit.aspx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science Coalition Tool-Kit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Science Coalition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established in 1994, the Science Coalition is a nonprofit, nonpartisan organization of more than 50 of the nation’s leading public and private research universities. It is dedicated to sustaining the federal government’s investment in basic scientific research as a means to stimulate the economy, spur innovation and drive America’s global competitiveness.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.sciencecoalition.org/mission-and-members</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvard GSAS Science Policy Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harvard University</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Harvard GSAS Science Policy Group is composed of graduate students interested in the intersection between science and policy. We work to engage Harvard science students by hosting networking events, chats with science policy experts, courses, career panels, local trips to government agencies, writing and research opportunities, and an annual visit to Washington, D.C.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://projects.iq.harvard.edu/sciencepolicy/home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIT Science Policy Initiative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The MIT Science Policy Initiative, founded in 2007, is a group of graduate (and some undergraduate) students who work closely with MIT Faculty, the MIT Washington DC Office, and other science policy advocates to better understand how scientists can play a central role in the framing of science and technology policy legislation and public discourse. We strive to create better scientists and engineers as well as a better society through rigorous research and authentic engagement with public policy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://mitspi.squarespace.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science and Education Policy Association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weill Cornell Medicine, The Rockefeller University, and Memorial Sloan Kettering Cancer Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Science &amp; Education Policy Association (SEPA) is a student-run organization founded at the Tri-Institute – Weill Cornell Medicine, The Rockefeller University, and Memorial Sloan Kettering Cancer Center – aiming to facilitate the interaction between scientists and the world of science policy. Launched in 2016 by Sarah Qamar and Dane Samilo, SEPA is continuing its work to advocate and raise awareness for the need for policy engagement within the scientific community.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://sepanyc.org/index.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fletcher Science Diplomacy Club</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tufts University, Fletcher School </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Fletcher Science Diplomacy club was founded in September 2016. It maintains close ties to the Science Diplomacy Center (Tufts University) and the Science Diplomacy Education Network (AAAS Center for Science Diplomacy). The club aims to raise awareness of the growing field of science diplomacy, highlighting the role of science in informing sound policy-making, solving global challenges and improving international relations. The club provides a forum for students, at the Fletcher School and beyond, to explore and understand issues at the intersection of science and international relations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://sites.tufts.edu/scidipclub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Science Policy Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of California, San Francisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are a registered campus organization (RCO) dedicated to educating our students and postdocs about science policy issues as well as taking action to support science advocacy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.facebook.com/UcsfSciencePolicyGroup</t>
   </si>
   <si>
     <t xml:space="preserve">AAAS R&amp;D Budget Dashboard</t>
@@ -1379,13 +1379,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.3953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.7023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="95.4976744186046"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.8093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="98.3255813953488"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,12 +1573,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="43.3162790697674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="55.2558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="113.711627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="56.8558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="117.153488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="48" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,87 +1600,87 @@
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="24" t="s">
         <v>240</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>241</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="24" t="s">
         <v>247</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>248</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="C5" s="24" t="s">
         <v>251</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>252</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="C6" s="24" t="s">
         <v>255</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>256</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -1710,9 +1710,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.6232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="115.553488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.2232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.4418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="119"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>33</v>
@@ -1729,7 +1729,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,7 +1737,7 @@
         <v>258</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>259</v>
@@ -1746,7 +1746,7 @@
         <v>260</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,7 +1763,7 @@
         <v>264</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1780,7 @@
         <v>267</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1797,7 @@
         <v>270</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -1824,10 +1824,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.5906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="36.7953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.5627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="37.7813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.2093023255814"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,23 +1987,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="9.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="15.1348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="67.1906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="15.506976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="9" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,19 +2171,6 @@
       <c r="I6" s="13" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2209,26 +2196,26 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="14" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="52.7953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="67.1906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="14" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="54.2697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="10" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="17" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>33</v>
@@ -2240,13 +2227,13 @@
         <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>67</v>
@@ -2257,114 +2244,114 @@
     </row>
     <row r="2" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>112</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>113</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>117</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>74</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>121</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>74</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2397,15 +2384,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.2232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="14" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="52.7953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="14" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="17.2279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="10" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="67.1906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="14" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="54.2697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="18" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="14" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="14" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="10" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="53" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2425,13 +2412,13 @@
         <v>64</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>65</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>66</v>
@@ -3456,32 +3443,32 @@
     </row>
     <row r="2" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>129</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
@@ -4500,34 +4487,34 @@
     </row>
     <row r="3" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="F3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="19" t="s">
         <v>129</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
@@ -5546,34 +5533,34 @@
     </row>
     <row r="4" customFormat="false" ht="41.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>140</v>
-      </c>
       <c r="F4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>129</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
@@ -6592,31 +6579,31 @@
     </row>
     <row r="5" s="23" customFormat="true" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>74</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J5" s="19" t="s">
         <v>74</v>
@@ -6652,12 +6639,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="61.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="69.6511627906977"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="71.7441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="26" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6665,7 +6652,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>33</v>
@@ -6679,104 +6666,104 @@
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>152</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>153</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="C5" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>162</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="C6" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="E6" s="24" t="s">
         <v>167</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="C7" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="D7" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -6806,11 +6793,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="24" width="62.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.15348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="104.604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="24" width="64.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="107.804651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="30" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6818,7 +6805,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>33</v>
@@ -6832,104 +6819,104 @@
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="31" t="s">
         <v>175</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>176</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>178</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>184</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>185</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>187</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>188</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="C7" s="31" t="s">
         <v>191</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>192</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>84</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -6956,13 +6943,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="74.2046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="87.9906976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="32" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="32" width="76.4232558139535"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="32" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="32" width="90.6976744186047"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="32" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="38" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6970,16 +6957,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>194</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>195</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>6</v>
@@ -6987,122 +6974,122 @@
     </row>
     <row r="2" s="39" customFormat="true" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="34" t="s">
+      <c r="F2" s="39" t="s">
         <v>198</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="F3" s="32" t="s">
         <v>203</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" s="32" t="s">
         <v>206</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" s="39" t="s">
+      <c r="D5" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>209</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="C6" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="D6" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="D6" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>214</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="C7" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>218</v>
-      </c>
       <c r="D7" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -7129,10 +7116,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="32" width="65.0976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="32" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="32" width="67.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="32" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="32" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="32" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7140,7 +7127,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C1" s="40" t="s">
         <v>33</v>
@@ -7151,72 +7138,72 @@
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="42" t="s">
+      <c r="D2" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C3" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="44" t="s">
         <v>226</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" s="43" t="s">
+      <c r="D4" s="44" t="s">
         <v>229</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="C5" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="D5" s="46" t="s">
         <v>233</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="C6" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="D6" s="32" t="s">
         <v>237</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>